<commit_message>
17 53 ssatinde doğru çalışan vue dosyası
</commit_message>
<xml_diff>
--- a/public/esmaulhusna.xlsx
+++ b/public/esmaulhusna.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ziyao\Desktop\Coding Projects\wordcardarabıc\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D005A1E-50A1-4144-B586-2996CB4F46A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE39BA1-45CB-466C-9978-509C2FA2FB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{530088D5-C0D1-4B54-9791-CDAD199E92DF}"/>
   </bookViews>
   <sheets>
     <sheet name="99İSMİ" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'99İSMİ'!$E$1:$E$101</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1042,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B14E0EA2-864E-4427-AE73-BA934C3F9A04}">
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="52.5"/>
@@ -1053,809 +1056,1013 @@
     <col min="1" max="1" width="41.375" style="3" customWidth="1"/>
     <col min="2" max="2" width="57.375" customWidth="1"/>
     <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35" customWidth="1"/>
+    <col min="5" max="5" width="33.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5" ht="69.75">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="69.75">
+      <c r="D1" s="4"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="69.75">
       <c r="A2" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="69.75">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="69.75">
       <c r="A3" s="4" t="s">
         <v>102</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="69.75">
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" ht="69.75">
       <c r="A4" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="69.75">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" ht="69.75">
       <c r="A5" s="4" t="s">
         <v>104</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="69.75">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="69.75">
       <c r="A6" s="4" t="s">
         <v>105</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="69.75">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" ht="69.75">
       <c r="A7" s="4" t="s">
         <v>106</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="69.75">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" ht="69.75">
       <c r="A8" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="69.75">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" ht="69.75">
       <c r="A9" s="4" t="s">
         <v>108</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="69.75">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="69.75">
       <c r="A10" s="4" t="s">
         <v>109</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="69.75">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="69.75">
       <c r="A11" s="4" t="s">
         <v>110</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="69.75">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" ht="69.75">
       <c r="A12" s="4" t="s">
         <v>111</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="69.75">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" ht="69.75">
       <c r="A13" s="4" t="s">
         <v>112</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="69.75">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" ht="69.75">
       <c r="A14" s="4" t="s">
         <v>113</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="69.75">
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" ht="69.75">
       <c r="A15" s="4" t="s">
         <v>114</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="69.75">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" ht="69.75">
       <c r="A16" s="4" t="s">
         <v>115</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="69.75">
+      <c r="D16" s="5"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="69.75">
       <c r="A17" s="4" t="s">
         <v>116</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="69.75">
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" ht="69.75">
       <c r="A18" s="4" t="s">
         <v>117</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="69.75">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" ht="69.75">
       <c r="A19" s="4" t="s">
         <v>118</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="69.75">
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" ht="69.75">
       <c r="A20" s="4" t="s">
         <v>119</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="69.75">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" ht="69.75">
       <c r="A21" s="4" t="s">
         <v>120</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="69.75">
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" ht="69.75">
       <c r="A22" s="4" t="s">
         <v>121</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="69.75">
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" ht="69.75">
       <c r="A23" s="4" t="s">
         <v>122</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="69.75">
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" ht="69.75">
       <c r="A24" s="4" t="s">
         <v>123</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="69.75">
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" ht="69.75">
       <c r="A25" s="4" t="s">
         <v>124</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="69.75">
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" ht="69.75">
       <c r="A26" s="4" t="s">
         <v>125</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="69.75">
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" ht="69.75">
       <c r="A27" s="4" t="s">
         <v>126</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="69.75">
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" ht="69.75">
       <c r="A28" s="4" t="s">
         <v>127</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="69.75">
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" ht="69.75">
       <c r="A29" s="4" t="s">
         <v>128</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="69.75">
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" ht="69.75">
       <c r="A30" s="4" t="s">
         <v>129</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="69.75">
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" ht="69.75">
       <c r="A31" s="4" t="s">
         <v>130</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="69.75">
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" ht="69.75">
       <c r="A32" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="69.75">
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" ht="69.75">
       <c r="A33" s="4" t="s">
         <v>132</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="69.75">
+      <c r="D33" s="5"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" ht="69.75">
       <c r="A34" s="4" t="s">
         <v>133</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="69.75">
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" ht="69.75">
       <c r="A35" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="69.75">
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" ht="69.75">
       <c r="A36" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="69.75">
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" ht="69.75">
       <c r="A37" s="4" t="s">
         <v>136</v>
       </c>
       <c r="B37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="69.75">
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" ht="69.75">
       <c r="A38" s="4" t="s">
         <v>137</v>
       </c>
       <c r="B38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="69.75">
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" ht="69.75">
       <c r="A39" s="4" t="s">
         <v>138</v>
       </c>
       <c r="B39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="69.75">
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" ht="69.75">
       <c r="A40" s="4" t="s">
         <v>139</v>
       </c>
       <c r="B40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="69.75">
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" ht="69.75">
       <c r="A41" s="4" t="s">
         <v>140</v>
       </c>
       <c r="B41" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="69.75">
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:5" ht="69.75">
       <c r="A42" s="4" t="s">
         <v>141</v>
       </c>
       <c r="B42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="69.75">
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:5" ht="69.75">
       <c r="A43" s="4" t="s">
         <v>142</v>
       </c>
       <c r="B43" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="69.75">
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:5" ht="69.75">
       <c r="A44" s="4" t="s">
         <v>143</v>
       </c>
       <c r="B44" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="69.75">
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:5" ht="69.75">
       <c r="A45" s="4" t="s">
         <v>144</v>
       </c>
       <c r="B45" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="69.75">
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="1:5" ht="69.75">
       <c r="A46" s="4" t="s">
         <v>145</v>
       </c>
       <c r="B46" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="69.75">
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="1:5" ht="69.75">
       <c r="A47" s="4" t="s">
         <v>146</v>
       </c>
       <c r="B47" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="69.75">
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="1:5" ht="69.75">
       <c r="A48" s="4" t="s">
         <v>147</v>
       </c>
       <c r="B48" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="69.75">
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:5" ht="69.75">
       <c r="A49" s="4" t="s">
         <v>148</v>
       </c>
       <c r="B49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="69.75">
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="1:5" ht="69.75">
       <c r="A50" s="4" t="s">
         <v>149</v>
       </c>
       <c r="B50" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="69.75">
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="1:5" ht="69.75">
       <c r="A51" s="4" t="s">
         <v>150</v>
       </c>
       <c r="B51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" ht="69.75">
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+    </row>
+    <row r="52" spans="1:5" ht="69.75">
       <c r="A52" s="4" t="s">
         <v>151</v>
       </c>
       <c r="B52" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="69.75">
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+    </row>
+    <row r="53" spans="1:5" ht="69.75">
       <c r="A53" s="4" t="s">
         <v>152</v>
       </c>
       <c r="B53" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" ht="69.75">
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+    </row>
+    <row r="54" spans="1:5" ht="69.75">
       <c r="A54" s="4" t="s">
         <v>153</v>
       </c>
       <c r="B54" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="69.75">
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+    </row>
+    <row r="55" spans="1:5" ht="69.75">
       <c r="A55" s="4" t="s">
         <v>154</v>
       </c>
       <c r="B55" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" ht="69.75">
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="1:5" ht="69.75">
       <c r="A56" s="4" t="s">
         <v>155</v>
       </c>
       <c r="B56" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" ht="69.75">
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="1:5" ht="69.75">
       <c r="A57" s="4" t="s">
         <v>156</v>
       </c>
       <c r="B57" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" ht="69.75">
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" spans="1:5" ht="69.75">
       <c r="A58" s="4" t="s">
         <v>157</v>
       </c>
       <c r="B58" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" ht="69.75">
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" spans="1:5" ht="69.75">
       <c r="A59" s="4" t="s">
         <v>158</v>
       </c>
       <c r="B59" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" ht="69.75">
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+    </row>
+    <row r="60" spans="1:5" ht="69.75">
       <c r="A60" s="4" t="s">
         <v>159</v>
       </c>
       <c r="B60" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" ht="69.75">
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="1:5" ht="69.75">
       <c r="A61" s="4" t="s">
         <v>160</v>
       </c>
       <c r="B61" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" ht="69.75">
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+    </row>
+    <row r="62" spans="1:5" ht="69.75">
       <c r="A62" s="4" t="s">
         <v>161</v>
       </c>
       <c r="B62" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" ht="69.75">
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+    </row>
+    <row r="63" spans="1:5" ht="69.75">
       <c r="A63" s="4" t="s">
         <v>162</v>
       </c>
       <c r="B63" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" ht="69.75">
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+    </row>
+    <row r="64" spans="1:5" ht="69.75">
       <c r="A64" s="4" t="s">
         <v>163</v>
       </c>
       <c r="B64" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" ht="69.75">
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+    </row>
+    <row r="65" spans="1:5" ht="69.75">
       <c r="A65" s="4" t="s">
         <v>164</v>
       </c>
       <c r="B65" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" ht="69.75">
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+    </row>
+    <row r="66" spans="1:5" ht="69.75">
       <c r="A66" s="4" t="s">
         <v>165</v>
       </c>
       <c r="B66" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" ht="69.75">
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="1:5" ht="69.75">
       <c r="A67" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B67" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" ht="69.75">
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="1:5" ht="69.75">
       <c r="A68" s="4" t="s">
         <v>167</v>
       </c>
       <c r="B68" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" ht="69.75">
+      <c r="D68" s="4"/>
+      <c r="E68" s="5"/>
+    </row>
+    <row r="69" spans="1:5" ht="69.75">
       <c r="A69" s="4" t="s">
         <v>168</v>
       </c>
       <c r="B69" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" ht="69.75">
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+    </row>
+    <row r="70" spans="1:5" ht="69.75">
       <c r="A70" s="4" t="s">
         <v>169</v>
       </c>
       <c r="B70" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" ht="69.75">
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+    </row>
+    <row r="71" spans="1:5" ht="69.75">
       <c r="A71" s="5" t="s">
         <v>170</v>
       </c>
       <c r="B71" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" ht="69.75">
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+    </row>
+    <row r="72" spans="1:5" ht="69.75">
       <c r="A72" s="4" t="s">
         <v>171</v>
       </c>
       <c r="B72" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" ht="69.75">
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+    </row>
+    <row r="73" spans="1:5" ht="69.75">
       <c r="A73" s="5" t="s">
         <v>172</v>
       </c>
       <c r="B73" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" ht="69.75">
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+    </row>
+    <row r="74" spans="1:5" ht="69.75">
       <c r="A74" s="4" t="s">
         <v>173</v>
       </c>
       <c r="B74" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" ht="69.75">
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+    </row>
+    <row r="75" spans="1:5" ht="69.75">
       <c r="A75" s="5" t="s">
         <v>174</v>
       </c>
       <c r="B75" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" ht="69.75">
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+    </row>
+    <row r="76" spans="1:5" ht="69.75">
       <c r="A76" s="4" t="s">
         <v>175</v>
       </c>
       <c r="B76" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" ht="69.75">
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+    </row>
+    <row r="77" spans="1:5" ht="69.75">
       <c r="A77" s="4" t="s">
         <v>176</v>
       </c>
       <c r="B77" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" ht="69.75">
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+    </row>
+    <row r="78" spans="1:5" ht="69.75">
       <c r="A78" s="4" t="s">
         <v>177</v>
       </c>
       <c r="B78" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" ht="69.75">
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+    </row>
+    <row r="79" spans="1:5" ht="69.75">
       <c r="A79" s="4" t="s">
         <v>178</v>
       </c>
       <c r="B79" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" ht="69.75">
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+    </row>
+    <row r="80" spans="1:5" ht="69.75">
       <c r="A80" s="4" t="s">
         <v>179</v>
       </c>
       <c r="B80" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" ht="69.75">
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+    </row>
+    <row r="81" spans="1:5" ht="69.75">
       <c r="A81" s="4" t="s">
         <v>180</v>
       </c>
       <c r="B81" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" ht="69.75">
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+    </row>
+    <row r="82" spans="1:5" ht="69.75">
       <c r="A82" s="4" t="s">
         <v>181</v>
       </c>
       <c r="B82" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" ht="69.75">
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+    </row>
+    <row r="83" spans="1:5" ht="69.75">
       <c r="A83" s="4" t="s">
         <v>182</v>
       </c>
       <c r="B83" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" ht="69.75">
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+    </row>
+    <row r="84" spans="1:5" ht="69.75">
       <c r="A84" s="4" t="s">
         <v>183</v>
       </c>
       <c r="B84" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" ht="69.75">
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+    </row>
+    <row r="85" spans="1:5" ht="69.75">
       <c r="A85" s="4" t="s">
         <v>184</v>
       </c>
       <c r="B85" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" ht="69.75">
+      <c r="D85" s="4"/>
+      <c r="E85" s="5"/>
+    </row>
+    <row r="86" spans="1:5" ht="69.75">
       <c r="A86" s="4" t="s">
         <v>185</v>
       </c>
       <c r="B86" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" ht="69.75">
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+    </row>
+    <row r="87" spans="1:5" ht="69.75">
       <c r="A87" s="4" t="s">
         <v>186</v>
       </c>
       <c r="B87" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" ht="69.75">
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+    </row>
+    <row r="88" spans="1:5" ht="69.75">
       <c r="A88" s="4" t="s">
         <v>187</v>
       </c>
       <c r="B88" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" ht="69.75">
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+    </row>
+    <row r="89" spans="1:5" ht="69.75">
       <c r="A89" s="4" t="s">
         <v>188</v>
       </c>
       <c r="B89" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" ht="69.75">
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+    </row>
+    <row r="90" spans="1:5" ht="69.75">
       <c r="A90" s="4" t="s">
         <v>189</v>
       </c>
       <c r="B90" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" ht="69.75">
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+    </row>
+    <row r="91" spans="1:5" ht="69.75">
       <c r="A91" s="4" t="s">
         <v>190</v>
       </c>
       <c r="B91" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" ht="69.75">
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
+    </row>
+    <row r="92" spans="1:5" ht="69.75">
       <c r="A92" s="4" t="s">
         <v>191</v>
       </c>
       <c r="B92" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" ht="69.75">
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
+    </row>
+    <row r="93" spans="1:5" ht="69.75">
       <c r="A93" s="4" t="s">
         <v>192</v>
       </c>
       <c r="B93" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" ht="69.75">
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+    </row>
+    <row r="94" spans="1:5" ht="69.75">
       <c r="A94" s="4" t="s">
         <v>193</v>
       </c>
       <c r="B94" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" ht="69.75">
+      <c r="D94" s="4"/>
+      <c r="E94" s="4"/>
+    </row>
+    <row r="95" spans="1:5" ht="69.75">
       <c r="A95" s="4" t="s">
         <v>194</v>
       </c>
       <c r="B95" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" ht="69.75">
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+    </row>
+    <row r="96" spans="1:5" ht="69.75">
       <c r="A96" s="4" t="s">
         <v>195</v>
       </c>
       <c r="B96" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" ht="69.75">
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
+    </row>
+    <row r="97" spans="1:5" ht="69.75">
       <c r="A97" s="4" t="s">
         <v>196</v>
       </c>
       <c r="B97" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" ht="69.75">
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+    </row>
+    <row r="98" spans="1:5" ht="69.75">
       <c r="A98" s="4" t="s">
         <v>197</v>
       </c>
       <c r="B98" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" ht="69.75">
+      <c r="D98" s="5"/>
+      <c r="E98" s="4"/>
+    </row>
+    <row r="99" spans="1:5" ht="69.75">
       <c r="A99" s="4" t="s">
         <v>198</v>
       </c>
       <c r="B99" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" ht="69.75">
+      <c r="D99" s="4"/>
+      <c r="E99" s="4"/>
+    </row>
+    <row r="100" spans="1:5" ht="69.75">
       <c r="A100" s="4" t="s">
         <v>199</v>
       </c>
       <c r="B100" t="s">
         <v>99</v>
       </c>
+      <c r="E100" s="4"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D1:D100">
+    <sortCondition descending="1" ref="D1:D100"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>